<commit_message>
added a real shoddy help menu...
</commit_message>
<xml_diff>
--- a/Layouts/Help Menu Layout.xlsx
+++ b/Layouts/Help Menu Layout.xlsx
@@ -48,13 +48,13 @@
     <t>Goal</t>
   </si>
   <si>
-    <t xml:space="preserve">Find your way through the labyrinthine purgatory to find the shattered pieces of your soul. Use your lighter sparingly and get around the beasts by either attacking them head on or utilizing traps and doors. </t>
-  </si>
-  <si>
-    <t>Time is Running Out</t>
-  </si>
-  <si>
-    <t>You are slowly becoming a beast. Being beast-like grants you heightened strength, but once you fully turn, you can never leave purgatory. Utilizing this extra strength speeds up the process as well.</t>
+    <t>Goal Body</t>
+  </si>
+  <si>
+    <t>Time Body</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -90,7 +90,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -98,6 +98,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,7 +406,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,153 +419,137 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="G8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="1"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="1"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="I8:J9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="A3:E10"/>
-    <mergeCell ref="F3:J6"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:E2"/>
+  <mergeCells count="7">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>